<commit_message>
Refined (corrected) tests and results
</commit_message>
<xml_diff>
--- a/cpu-test-freemarker.xlsx
+++ b/cpu-test-freemarker.xlsx
@@ -17,19 +17,25 @@
   </pivotCaches>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1565707733" val="966" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1565707733" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1565707733" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1565707733"/>
+      <pm:revision xmlns:pm="smNativeData" day="1566329169" val="966" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1566329169" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1566329169" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1566329169"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
-    <t>1,000,000 events</t>
+    <t>100,000 events</t>
+  </si>
+  <si>
+    <t>FreeMarker</t>
+  </si>
+  <si>
+    <t>JSLT</t>
   </si>
   <si>
     <t>CPUs</t>
@@ -51,7 +57,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
+  <numFmts count="8">
     <numFmt numFmtId="5" formatCode="#,##0\ &quot;$&quot;;\-#,##0\ &quot;$&quot;"/>
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;$&quot;;[Red]\-#,##0\ &quot;$&quot;"/>
     <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;$&quot;;\-#,##0.00\ &quot;$&quot;"/>
@@ -60,9 +66,8 @@
     <numFmt numFmtId="41" formatCode="_-* #,##0\ _$_-;\-* #,##0\ _$_-;_-* &quot;-&quot;\ _$_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
-    <numFmt numFmtId="3" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <name val="Arial"/>
       <family val="1"/>
@@ -70,7 +75,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1565707733" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1566329169" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -85,24 +90,10 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1565707733" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1566329169" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Monospace"/>
-      <color rgb="FFFF0000"/>
-      <sz val="10"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1565707733" fgClr="FF0000" ulstyle="none">
-            <pm:latin face="Monospace" sz="200" lang="default"/>
-            <pm:cs face="Basic Sans" sz="200" lang="default"/>
-            <pm:ea face="Basic Sans" sz="200" lang="default"/>
           </pm:charSpec>
         </ext>
       </extLst>
@@ -113,7 +104,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1565707733" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1566329169" ulstyle="none" kern="1">
             <pm:latin face="Monospace" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -127,7 +118,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1565707733" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1566329169" ulstyle="none">
             <pm:latin face="Monospace" sz="200" lang="default"/>
             <pm:cs face="Basic Sans" sz="200" lang="default"/>
             <pm:ea face="Basic Sans" sz="200" lang="default"/>
@@ -136,7 +127,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,7 +143,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1565707733" type="1" fgLvl="100" fgClr="00DCE6F1" bgLvl="100" bgClr="00DCE6F1"/>
+            <pm:shade xmlns:pm="smNativeData" id="1566329169" type="1" fgLvl="100" fgClr="00DCE6F1" bgLvl="100" bgClr="00DCE6F1"/>
           </ext>
         </extLst>
       </patternFill>
@@ -166,13 +157,24 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1565707733" type="1" fgLvl="100" fgClr="00DCE6F1" bgLvl="100" bgClr="00DCE6F1"/>
+            <pm:shade xmlns:pm="smNativeData" id="1566329169" type="1" fgLvl="100" fgClr="00DCE6F1" bgLvl="100" bgClr="00DCE6F1"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1566329169" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -188,7 +190,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565707733"/>
+          <pm:border xmlns:pm="smNativeData" id="1566329169"/>
         </ext>
       </extLst>
     </border>
@@ -207,7 +209,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565707733">
+          <pm:border xmlns:pm="smNativeData" id="1566329169">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="95B3D7"/>
           </pm:border>
         </ext>
@@ -228,7 +230,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565707733">
+          <pm:border xmlns:pm="smNativeData" id="1566329169">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="95B3D7"/>
           </pm:border>
         </ext>
@@ -249,7 +251,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565707733">
+          <pm:border xmlns:pm="smNativeData" id="1566329169">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="95B3D7"/>
           </pm:border>
         </ext>
@@ -270,9 +272,28 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565707733">
+          <pm:border xmlns:pm="smNativeData" id="1566329169">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="95B3D7"/>
           </pm:border>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1566329169"/>
         </ext>
       </extLst>
     </border>
@@ -280,13 +301,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -294,10 +312,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1565707733" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1566329169" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1565707733" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1566329169" count="5">
         <pm:color name="Color 24" rgb="95B3D7"/>
         <pm:color name="Color 25" rgb="DCE6F1"/>
         <pm:color name="Color 26" rgb="D8D8D8"/>
@@ -324,94 +342,150 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>millis</c:v>
+            <c:v>FreeMarker</c:v>
           </c:tx>
-          <c:cat>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$16</c:f>
+              <c:f>Sheet1!$B$6:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>33035</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>17722</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>13222</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>10928</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>9549</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>8164</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>8382</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>7735</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>7789</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>7645</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>7280</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>7634</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:sm="smo" uri="smo">
+              <sm:meanLine>
+                <c:spPr>
+                  <a:ln w="9525">
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+              </sm:meanLine>
+              <sm:minMaxLine>
+                <c:spPr>
+                  <a:ln w="9525">
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+              </sm:minMaxLine>
+              <sm:stDevLine>
+                <c:spPr>
+                  <a:ln w="9525">
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+              </sm:stDevLine>
+              <sm:trendLine>
+                <c:spPr>
+                  <a:ln w="9525">
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+              </sm:trendLine>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>JSLT</c:v>
+          </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$16</c:f>
+              <c:f>Sheet1!$C$6:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>35705</c:v>
+                  <c:v>11577</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18917</c:v>
+                  <c:v>6870</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13514</c:v>
+                  <c:v>5018</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11405</c:v>
+                  <c:v>4149</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9108</c:v>
+                  <c:v>3588</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8172</c:v>
+                  <c:v>3676</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7781</c:v>
+                  <c:v>3381</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7965</c:v>
+                  <c:v>3629</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7394</c:v>
+                  <c:v>3432</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7753</c:v>
+                  <c:v>3625</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7662</c:v>
+                  <c:v>3400</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7222</c:v>
+                  <c:v>3446</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -483,7 +557,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-us" sz="1210" b="1" i="0" u="none" strike="noStrike" kern="100">
+                  <a:defRPr lang="en-us" sz="1365" b="1" i="0" u="none" strike="noStrike" kern="100">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -499,7 +573,7 @@
           <c:layout/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="9525">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -508,6 +582,20 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-us" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="100">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Basic Sans" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="11"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -527,7 +615,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-us" sz="1210" b="1" i="0" u="none" strike="noStrike" kern="100">
+                  <a:defRPr lang="en-us" sz="1365" b="1" i="0" u="none" strike="noStrike" kern="100">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -543,7 +631,7 @@
           <c:layout/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="9525">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -552,6 +640,20 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-us" sz="900" b="0" i="0" u="none" strike="noStrike" kern="100">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Basic Sans" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="10"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -585,7 +687,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr lang="en-us" sz="1210" b="0" i="0" u="none" strike="noStrike" kern="100">
+        <a:defRPr lang="en-us" sz="1365" b="0" i="0" u="none" strike="noStrike" kern="100">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
@@ -596,7 +698,7 @@
   </c:txPr>
   <c:extLst>
     <c:ext xmlns:sm="smo" uri="smo">
-      <sm:colorScheme xmlns:sm="smo" id="1565707733" val="7"/>
+      <sm:colorScheme xmlns:sm="smo" id="1566329169" val="7"/>
     </c:ext>
   </c:extLst>
 </c:chartSpace>
@@ -607,15 +709,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>132715</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>123190</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -640,7 +742,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="12">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A4:B16" sheet="Sheet1"/>
+    <worksheetSource ref="A5:B17" sheet="Sheet1"/>
   </cacheSource>
   <cacheFields count="2">
     <cacheField name="CPUs" numFmtId="0">
@@ -1042,10 +1144,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:B31"/>
+  <dimension ref="A2:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -1055,211 +1157,163 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4"/>
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="n">
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>35705</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="n">
+      <c r="B6" s="1" t="n">
+        <v>33035</v>
+      </c>
+      <c r="C6" t="n">
+        <v>11577</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>18917</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="n">
+      <c r="B7" s="1" t="n">
+        <v>17722</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6870</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>13514</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="n">
+      <c r="B8" s="1" t="n">
+        <v>13222</v>
+      </c>
+      <c r="C8" t="n">
+        <v>5018</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="n">
-        <v>11405</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="n">
+      <c r="B9" s="1" t="n">
+        <v>10928</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <v>9108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="n">
+      <c r="B10" s="1" t="n">
+        <v>9549</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3588</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="1" t="n">
-        <v>8172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="n">
+      <c r="B11" s="1" t="n">
+        <v>8164</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3676</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="n">
         <v>7</v>
       </c>
-      <c r="B11" s="1" t="n">
-        <v>7781</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="n">
+      <c r="B12" s="1" t="n">
+        <v>8382</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3381</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="n">
         <v>8</v>
       </c>
-      <c r="B12" s="2" t="n">
-        <v>7965</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="n">
+      <c r="B13" s="2" t="n">
+        <v>7735</v>
+      </c>
+      <c r="C13" t="n">
+        <v>3629</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="n">
         <v>9</v>
       </c>
-      <c r="B13" s="2" t="n">
-        <v>7394</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="n">
+      <c r="B14" s="2" t="n">
+        <v>7789</v>
+      </c>
+      <c r="C14" t="n">
+        <v>3432</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="n">
         <v>10</v>
       </c>
-      <c r="B14" s="2" t="n">
-        <v>7753</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="n">
+      <c r="B15" s="2" t="n">
+        <v>7645</v>
+      </c>
+      <c r="C15" t="n">
+        <v>3625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="n">
         <v>11</v>
       </c>
-      <c r="B15" s="2" t="n">
-        <v>7662</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="n">
+      <c r="B16" s="2" t="n">
+        <v>7280</v>
+      </c>
+      <c r="C16" t="n">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="n">
         <v>12</v>
       </c>
-      <c r="B16" s="2" t="n">
-        <v>7222</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="n">
-        <v>1</v>
-      </c>
-      <c r="B20" s="3" t="n">
-        <v>36616</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="n">
-        <v>2</v>
-      </c>
-      <c r="B21" s="3" t="n">
-        <v>20199</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="n">
-        <v>3</v>
-      </c>
-      <c r="B22" s="3" t="n">
-        <v>13809</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="n">
-        <v>4</v>
-      </c>
-      <c r="B23" s="3" t="n">
-        <v>10945</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="n">
-        <v>5</v>
-      </c>
-      <c r="B24" s="3" t="n">
-        <v>9504</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="n">
-        <v>6</v>
-      </c>
-      <c r="B25" s="3" t="n">
-        <v>8134</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="n">
-        <v>7</v>
-      </c>
-      <c r="B26" s="3" t="n">
-        <v>8116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="n">
-        <v>8</v>
-      </c>
-      <c r="B27" s="3" t="n">
-        <v>7759</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="n">
-        <v>9</v>
-      </c>
-      <c r="B28" s="3" t="n">
-        <v>7530</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="n">
-        <v>10</v>
-      </c>
-      <c r="B29" s="3" t="n">
-        <v>7582</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="n">
-        <v>11</v>
-      </c>
-      <c r="B30" s="3" t="n">
-        <v>7208</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="n">
-        <v>12</v>
-      </c>
-      <c r="B31" s="3" t="n">
-        <v>7436</v>
+      <c r="B17" s="2" t="n">
+        <v>7634</v>
+      </c>
+      <c r="C17" t="n">
+        <v>3446</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1565707733" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1566329169" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1268,15 +1322,15 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1565707733" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1565707733" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1566329169" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1566329169" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <drawing r:id="rId1"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1565707733" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1566329169" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1301,10 +1355,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1405,7 +1459,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B14" t="n">
         <v>142598</v>
@@ -1415,7 +1469,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1565707733" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1566329169" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1424,14 +1478,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1565707733" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1565707733" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1566329169" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1566329169" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1565707733" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1566329169" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
FreeMarker optimization and new performance test
</commit_message>
<xml_diff>
--- a/cpu-test-freemarker.xlsx
+++ b/cpu-test-freemarker.xlsx
@@ -17,10 +17,10 @@
   </pivotCaches>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1566512357" val="966" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1566512357" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1566512357" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1566512357"/>
+      <pm:revision xmlns:pm="smNativeData" day="1566564940" val="966" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1566564940" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1566564940" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1566564940"/>
     </ext>
   </extLst>
 </workbook>
@@ -57,7 +57,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
+  <numFmts count="10">
     <numFmt numFmtId="5" formatCode="#,##0\ &quot;$&quot;;\-#,##0\ &quot;$&quot;"/>
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;$&quot;;[Red]\-#,##0\ &quot;$&quot;"/>
     <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;$&quot;;\-#,##0.00\ &quot;$&quot;"/>
@@ -67,6 +67,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
     <numFmt numFmtId="1" formatCode="0"/>
+    <numFmt numFmtId="10" formatCode="0.00%"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -76,7 +77,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1566512357" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1566564940" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -91,7 +92,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1566512357" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1566564940" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -105,7 +106,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1566512357" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1566564940" ulstyle="none" kern="1">
             <pm:latin face="Monospace" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -119,7 +120,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1566512357" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1566564940" ulstyle="none">
             <pm:latin face="Monospace" sz="200" lang="default"/>
             <pm:cs face="Basic Sans" sz="200" lang="default"/>
             <pm:ea face="Basic Sans" sz="200" lang="default"/>
@@ -144,7 +145,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1566512357" type="1" fgLvl="100" fgClr="00DCE6F1" bgLvl="100" bgClr="00DCE6F1"/>
+            <pm:shade xmlns:pm="smNativeData" id="1566564940" type="1" fgLvl="100" fgClr="00DCE6F1" bgLvl="100" bgClr="00DCE6F1"/>
           </ext>
         </extLst>
       </patternFill>
@@ -158,7 +159,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1566512357" type="1" fgLvl="100" fgClr="00DCE6F1" bgLvl="100" bgClr="00DCE6F1"/>
+            <pm:shade xmlns:pm="smNativeData" id="1566564940" type="1" fgLvl="100" fgClr="00DCE6F1" bgLvl="100" bgClr="00DCE6F1"/>
           </ext>
         </extLst>
       </patternFill>
@@ -169,7 +170,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1566512357" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1566564940" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -191,7 +192,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1566512357"/>
+          <pm:border xmlns:pm="smNativeData" id="1566564940"/>
         </ext>
       </extLst>
     </border>
@@ -210,7 +211,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1566512357">
+          <pm:border xmlns:pm="smNativeData" id="1566564940">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="95B3D7"/>
           </pm:border>
         </ext>
@@ -231,7 +232,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1566512357">
+          <pm:border xmlns:pm="smNativeData" id="1566564940">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="95B3D7"/>
           </pm:border>
         </ext>
@@ -252,7 +253,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1566512357">
+          <pm:border xmlns:pm="smNativeData" id="1566564940">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="95B3D7"/>
           </pm:border>
         </ext>
@@ -273,7 +274,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1566512357">
+          <pm:border xmlns:pm="smNativeData" id="1566564940">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="95B3D7"/>
           </pm:border>
         </ext>
@@ -294,7 +295,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1566512357"/>
+          <pm:border xmlns:pm="smNativeData" id="1566564940"/>
         </ext>
       </extLst>
     </border>
@@ -302,11 +303,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -314,10 +316,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1566512357" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1566564940" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1566512357" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1566564940" count="5">
         <pm:color name="Color 24" rgb="95B3D7"/>
         <pm:color name="Color 25" rgb="DCE6F1"/>
         <pm:color name="Color 26" rgb="D8D8D8"/>
@@ -369,40 +371,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>32107</c:v>
+                  <c:v>31977</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17176</c:v>
+                  <c:v>16956</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12546</c:v>
+                  <c:v>11649</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10188</c:v>
+                  <c:v>9833</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9192</c:v>
+                  <c:v>8732</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7705</c:v>
+                  <c:v>7754</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7416</c:v>
+                  <c:v>7269</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7522</c:v>
+                  <c:v>6988</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7266</c:v>
+                  <c:v>6887</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6931</c:v>
+                  <c:v>7096</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7164</c:v>
+                  <c:v>7196</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6774</c:v>
+                  <c:v>6719</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -454,40 +456,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>15682</c:v>
+                  <c:v>15639</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8570</c:v>
+                  <c:v>8266</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6457</c:v>
+                  <c:v>6411</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5481</c:v>
+                  <c:v>6182</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5802</c:v>
+                  <c:v>5752</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5379</c:v>
+                  <c:v>5441</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5709</c:v>
+                  <c:v>5422</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5800</c:v>
+                  <c:v>5785</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5473</c:v>
+                  <c:v>5501</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5917</c:v>
+                  <c:v>5667</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6036</c:v>
+                  <c:v>5852</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5926</c:v>
+                  <c:v>5699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -700,7 +702,7 @@
   </c:txPr>
   <c:extLst>
     <c:ext xmlns:sm="smo" uri="smo">
-      <sm:colorScheme xmlns:sm="smo" id="1566512357" val="7"/>
+      <sm:colorScheme xmlns:sm="smo" id="1566564940" val="7"/>
     </c:ext>
   </c:extLst>
 </c:chartSpace>
@@ -710,14 +712,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>29210</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>132715</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -1146,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C21"/>
+  <dimension ref="A2:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -1159,8 +1161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4"/>
+    <row r="4" spans="2:3">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -1179,153 +1180,201 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" t="n">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>32107</v>
+        <v>31977</v>
       </c>
       <c r="C6" t="n">
-        <v>15682</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>15639</v>
+      </c>
+      <c r="D6" s="4">
+        <f>(B6-C6)/B6</f>
+        <v>0.510929730743972144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="n">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>17176</v>
+        <v>16956</v>
       </c>
       <c r="C7" t="n">
-        <v>8570</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>8266</v>
+      </c>
+      <c r="D7" s="4">
+        <f>(B7-C7)/B7</f>
+        <v>0.512502948808681325</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="n">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>12546</v>
+        <v>11649</v>
       </c>
       <c r="C8" t="n">
-        <v>6457</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>6411</v>
+      </c>
+      <c r="D8" s="4">
+        <f>(B8-C8)/B8</f>
+        <v>0.449652330672160705</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="n">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>10188</v>
+        <v>9833</v>
       </c>
       <c r="C9" t="n">
-        <v>5481</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>6182</v>
+      </c>
+      <c r="D9" s="4">
+        <f>(B9-C9)/B9</f>
+        <v>0.371300722058374832</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="n">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>9192</v>
+        <v>8732</v>
       </c>
       <c r="C10" t="n">
-        <v>5802</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>5752</v>
+      </c>
+      <c r="D10" s="4">
+        <f>(B10-C10)/B10</f>
+        <v>0.341273476866697179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="n">
         <v>6</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>7705</v>
+        <v>7754</v>
       </c>
       <c r="C11" t="n">
-        <v>5379</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>5441</v>
+      </c>
+      <c r="D11" s="4">
+        <f>(B11-C11)/B11</f>
+        <v>0.298297652824348702</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="n">
         <v>7</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>7416</v>
+        <v>7269</v>
       </c>
       <c r="C12" t="n">
-        <v>5709</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>5422</v>
+      </c>
+      <c r="D12" s="4">
+        <f>(B12-C12)/B12</f>
+        <v>0.254092722520291625</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="n">
         <v>8</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>7522</v>
+        <v>6988</v>
       </c>
       <c r="C13" t="n">
-        <v>5800</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>5785</v>
+      </c>
+      <c r="D13" s="4">
+        <f>(B13-C13)/B13</f>
+        <v>0.172152261018889519</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="n">
         <v>9</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>7266</v>
+        <v>6887</v>
       </c>
       <c r="C14" t="n">
-        <v>5473</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>5501</v>
+      </c>
+      <c r="D14" s="4">
+        <f>(B14-C14)/B14</f>
+        <v>0.201248729490344136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="n">
         <v>10</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>6931</v>
+        <v>7096</v>
       </c>
       <c r="C15" t="n">
-        <v>5917</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>5667</v>
+      </c>
+      <c r="D15" s="4">
+        <f>(B15-C15)/B15</f>
+        <v>0.201381059751972913</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="n">
         <v>11</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>7164</v>
+        <v>7196</v>
       </c>
       <c r="C16" t="n">
-        <v>6036</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>5852</v>
+      </c>
+      <c r="D16" s="4">
+        <f>(B16-C16)/B16</f>
+        <v>0.186770428015564214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="n">
         <v>12</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>6774</v>
+        <v>6719</v>
       </c>
       <c r="C17" t="n">
-        <v>5926</v>
+        <v>5699</v>
+      </c>
+      <c r="D17" s="4">
+        <f>(B17-C17)/B17</f>
+        <v>0.151808304807262973</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="B21" s="3">
         <f>1000000/B17*1000</f>
-        <v>147623.265426630998</v>
+        <v>148831.671379670006</v>
       </c>
       <c r="C21" s="3">
-        <f>1000000/C11*1000</f>
-        <v>185908.161368283996</v>
+        <f>1000000/C12*1000</f>
+        <v>184433.78827001102</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1566512357" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1566564940" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1334,15 +1383,15 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1566512357" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1566512357" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1566564940" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1566564940" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <drawing r:id="rId1"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1566512357" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1566564940" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1481,7 +1530,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1566512357" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1566564940" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1490,14 +1539,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1566512357" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1566512357" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1566564940" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1566564940" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1566512357" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1566564940" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>